<commit_message>
Dynamic Max DMSO % in Echo spotting
</commit_message>
<xml_diff>
--- a/frontend/order_template.xlsx
+++ b/frontend/order_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
   <si>
     <t xml:space="preserve">Compound Id</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t xml:space="preserve">DMSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max DMSO percent:</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
@@ -452,11 +455,11 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="16.38"/>
@@ -544,13 +547,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB25"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="12.44"/>
@@ -568,6 +571,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="4" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="22" style="4" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="4" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="18.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,16 +696,22 @@
       <c r="AB2" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="AC2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>10</v>
@@ -718,27 +728,27 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA4" s="14" t="s">
-        <v>12</v>
-      </c>
       <c r="AB4" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -756,18 +766,18 @@
         <v>9</v>
       </c>
       <c r="AB5" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="X6" s="10" t="s">
         <v>10</v>
@@ -778,7 +788,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>8</v>
@@ -792,7 +802,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>8</v>
@@ -806,7 +816,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>8</v>
@@ -823,13 +833,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="X10" s="10" t="s">
         <v>10</v>
@@ -840,7 +850,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>8</v>
@@ -854,7 +864,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -868,7 +878,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>8</v>
@@ -882,7 +892,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>8</v>
@@ -899,13 +909,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>10</v>
@@ -916,7 +926,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>8</v>
@@ -930,7 +940,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Move max DMSO volume from Excel to a edit box
</commit_message>
<xml_diff>
--- a/frontend/order_template.xlsx
+++ b/frontend/order_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="29">
   <si>
     <t xml:space="preserve">Compound Id</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">DMSO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max DMSO percent:</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
@@ -459,7 +456,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="16.38"/>
@@ -547,13 +544,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD25"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="12.44"/>
@@ -696,22 +693,16 @@
       <c r="AB2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AC2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD2" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>13</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>10</v>
@@ -728,27 +719,27 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -766,18 +757,18 @@
         <v>9</v>
       </c>
       <c r="AB5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X6" s="10" t="s">
         <v>10</v>
@@ -788,7 +779,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>8</v>
@@ -802,7 +793,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>8</v>
@@ -816,7 +807,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>8</v>
@@ -833,13 +824,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X10" s="10" t="s">
         <v>10</v>
@@ -850,7 +841,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>8</v>
@@ -864,7 +855,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -878,7 +869,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>8</v>
@@ -892,7 +883,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>8</v>
@@ -909,13 +900,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>10</v>
@@ -926,7 +917,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>8</v>
@@ -940,7 +931,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>8</v>

</xml_diff>